<commit_message>
release silkscreen corrections, diode added
</commit_message>
<xml_diff>
--- a/Project Outputs/BOM/Bill of Materials-BOM.xlsx
+++ b/Project Outputs/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\UAVCAN-Sniffer-STM-Programmer\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{208CF297-42DA-4FC4-B118-64CEBC220DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C4D7968-9C94-4EFB-A4D6-5B02F57B7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{2CC9C527-FC56-438C-ADE5-247B22C17051}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{72C52343-086D-4B67-97BC-867CE1B797FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="148">
   <si>
     <t>Designator</t>
   </si>
@@ -184,6 +184,21 @@
   </si>
   <si>
     <t>0603-LED-BLUE</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Taiwan Semiconductor</t>
+  </si>
+  <si>
+    <t>SMAJ5.0</t>
+  </si>
+  <si>
+    <t>DO-214AC-2 Taiwan Semiconductor</t>
+  </si>
+  <si>
+    <t>400W, 6.9V, 10%, Unidirectional, TVS</t>
   </si>
   <si>
     <t>D3</t>
@@ -842,8 +857,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A2A316-472C-41AA-BCD7-D6A055264C00}">
-  <dimension ref="A1:L24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F72B815-BFD7-476D-9292-E040568D547B}">
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1112,160 +1127,150 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="1">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1276,138 +1281,144 @@
         <v>80</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="1">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2" t="s">
@@ -1416,245 +1427,247 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="2" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="K18" s="2" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="I19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1"/>
+      <c r="K19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="L19" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="1"/>
+      <c r="I22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="L22" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="I23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="K23" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="L23" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1662,37 +1675,67 @@
         <v>136</v>
       </c>
       <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>138</v>
+      <c r="D25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with 2 mosfets
</commit_message>
<xml_diff>
--- a/Project Outputs/BOM/Bill of Materials-BOM.xlsx
+++ b/Project Outputs/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\UAVCAN-Sniffer-STM-Programmer\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0242EE6-1545-4D5B-8320-E759E01B7F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBE70765-F898-4594-9F6F-B213E3ABFE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{411E2F86-ECC4-4043-B929-902B9FDBC9CF}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{20DFB516-F2F3-4B47-81AA-ACF1EF58501B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="147">
   <si>
     <t>Designator</t>
   </si>
@@ -225,6 +225,33 @@
     <t>SM10B-SRSS-TB</t>
   </si>
   <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Infineon</t>
+  </si>
+  <si>
+    <t>IRF5852</t>
+  </si>
+  <si>
+    <t>Mosfet Array 2 N-Channel _Dual_ 20V 2.7A 960mW Surface Mount 6-TSOP</t>
+  </si>
+  <si>
+    <t>TSOP-6 International Rectifier</t>
+  </si>
+  <si>
+    <t>https://static.chipdip.ru/lib/300/DOC000300076.pdf</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>IRF5850</t>
+  </si>
+  <si>
+    <t>Mosfet Array 2 P-Channel (Dual) 20V 2.2A 960mW Surface Mount 6-TSOP</t>
+  </si>
+  <si>
     <t>R1, R2, R3, R10, R11, R12</t>
   </si>
   <si>
@@ -270,7 +297,7 @@
     <t>120</t>
   </si>
   <si>
-    <t>R6, R7, R9, R13, R15, R17, R24</t>
+    <t>R6, R7, R9, R13, R15, R17, R18, R19, R24</t>
   </si>
   <si>
     <t>RC0402FR-0710KL</t>
@@ -827,8 +854,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A88DF1-3BAF-42EA-B7BA-959B89AB519C}">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9250EE5C-1A80-478A-8F44-C77F69EF6399}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1191,7 +1218,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>63</v>
@@ -1202,121 +1229,107 @@
       <c r="E12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="H14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="J14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>18</v>
@@ -1324,60 +1337,56 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="I16" s="1"/>
       <c r="J16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>17</v>
@@ -1386,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>18</v>
@@ -1394,75 +1403,83 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="J18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="J19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K19" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>99</v>
@@ -1470,14 +1487,18 @@
       <c r="E20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="2" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="K20" s="1"/>
     </row>
@@ -1486,215 +1507,273 @@
         <v>102</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="I21" s="1"/>
       <c r="J21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="G23" s="2" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="J23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>126</v>
-      </c>
+      <c r="I25" s="1"/>
       <c r="J25" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="H26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="1">
+      <c r="F27" s="1"/>
+      <c r="G27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>